<commit_message>
updated TZA and LKA to allow for running with new model
</commit_message>
<xml_diff>
--- a/article_6_tanzania_sri_lanka_peru/transformations_peru/templates/calibrated/peru/model_input_variables_peru_se_calibrated.xlsx
+++ b/article_6_tanzania_sri_lanka_peru/transformations_peru/templates/calibrated/peru/model_input_variables_peru_se_calibrated.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
-    <sheet name="strategy_id-6000" sheetId="2" r:id="rId2"/>
+    <sheet name="strategy_id-6002" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -1076,9 +1076,6 @@
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6">
-        <v>13</v>
-      </c>
       <c r="H6">
         <v>1</v>
       </c>
@@ -2083,9 +2080,6 @@
       <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="C2">
-        <v>13</v>
-      </c>
       <c r="H2">
         <v>1</v>
       </c>
@@ -2111,91 +2105,91 @@
         <v>0.95</v>
       </c>
       <c r="P2">
-        <v>0.9399999999999999</v>
+        <v>0.9253333333333333</v>
       </c>
       <c r="Q2">
-        <v>0.93</v>
+        <v>0.9013333333333334</v>
       </c>
       <c r="R2">
-        <v>0.92</v>
+        <v>0.8780000000000001</v>
       </c>
       <c r="S2">
-        <v>0.91</v>
+        <v>0.8553333333333334</v>
       </c>
       <c r="T2">
-        <v>0.9</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="U2">
-        <v>0.89</v>
+        <v>0.8120000000000001</v>
       </c>
       <c r="V2">
-        <v>0.88</v>
+        <v>0.7913333333333333</v>
       </c>
       <c r="W2">
-        <v>0.8539130434782609</v>
+        <v>0.7713333333333333</v>
       </c>
       <c r="X2">
-        <v>0.8286956521739131</v>
+        <v>0.752</v>
       </c>
       <c r="Y2">
-        <v>0.8043478260869564</v>
+        <v>0.7333333333333334</v>
       </c>
       <c r="Z2">
-        <v>0.7808695652173914</v>
+        <v>0.7153333333333333</v>
       </c>
       <c r="AA2">
-        <v>0.7582608695652174</v>
+        <v>0.698</v>
       </c>
       <c r="AB2">
-        <v>0.7365217391304347</v>
+        <v>0.6813333333333333</v>
       </c>
       <c r="AC2">
-        <v>0.7156521739130435</v>
+        <v>0.6653333333333333</v>
       </c>
       <c r="AD2">
-        <v>0.6956521739130435</v>
+        <v>0.65</v>
       </c>
       <c r="AE2">
-        <v>0.6765217391304349</v>
+        <v>0.6353333333333333</v>
       </c>
       <c r="AF2">
-        <v>0.6582608695652175</v>
+        <v>0.6213333333333333</v>
       </c>
       <c r="AG2">
-        <v>0.6408695652173912</v>
+        <v>0.6080000000000001</v>
       </c>
       <c r="AH2">
-        <v>0.6243478260869566</v>
+        <v>0.5953333333333333</v>
       </c>
       <c r="AI2">
-        <v>0.6086956521739131</v>
+        <v>0.5833333333333333</v>
       </c>
       <c r="AJ2">
-        <v>0.5939130434782609</v>
+        <v>0.5720000000000001</v>
       </c>
       <c r="AK2">
-        <v>0.5800000000000001</v>
+        <v>0.5613333333333334</v>
       </c>
       <c r="AL2">
-        <v>0.5669565217391305</v>
+        <v>0.5513333333333333</v>
       </c>
       <c r="AM2">
-        <v>0.5547826086956522</v>
+        <v>0.542</v>
       </c>
       <c r="AN2">
-        <v>0.5434782608695652</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="AO2">
-        <v>0.5347826086956522</v>
+        <v>0.5266666666666666</v>
       </c>
       <c r="AP2">
-        <v>0.5260869565217391</v>
+        <v>0.52</v>
       </c>
       <c r="AQ2">
-        <v>0.5173913043478261</v>
+        <v>0.5133333333333333</v>
       </c>
       <c r="AR2">
-        <v>0.508695652173913</v>
+        <v>0.5066666666666667</v>
       </c>
       <c r="AS2">
         <v>0.5</v>

</xml_diff>

<commit_message>
updated builds of regional input files
</commit_message>
<xml_diff>
--- a/article_6_tanzania_sri_lanka_peru/transformations_peru/templates/calibrated/peru/model_input_variables_peru_se_calibrated.xlsx
+++ b/article_6_tanzania_sri_lanka_peru/transformations_peru/templates/calibrated/peru/model_input_variables_peru_se_calibrated.xlsx
@@ -9,13 +9,22 @@
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
     <sheet name="strategy_id-6002" sheetId="2" r:id="rId2"/>
+    <sheet name="strategy_id-6003" sheetId="3" r:id="rId3"/>
+    <sheet name="strategy_id-6004" sheetId="4" r:id="rId4"/>
+    <sheet name="strategy_id-6005" sheetId="5" r:id="rId5"/>
+    <sheet name="strategy_id-6006" sheetId="6" r:id="rId6"/>
+    <sheet name="strategy_id-6007" sheetId="7" r:id="rId7"/>
+    <sheet name="strategy_id-6008" sheetId="8" r:id="rId8"/>
+    <sheet name="strategy_id-6009" sheetId="9" r:id="rId9"/>
+    <sheet name="strategy_id-6010" sheetId="10" r:id="rId10"/>
+    <sheet name="strategy_id-6011" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="58">
   <si>
     <t>subsector</t>
   </si>
@@ -23,18 +32,18 @@
     <t>variable</t>
   </si>
   <si>
+    <t>normalize_group</t>
+  </si>
+  <si>
+    <t>trajgroup_no_vary_q</t>
+  </si>
+  <si>
+    <t>uniform_scaling_q</t>
+  </si>
+  <si>
     <t>variable_trajectory_group</t>
   </si>
   <si>
-    <t>normalize_group</t>
-  </si>
-  <si>
-    <t>trajgroup_no_vary_q</t>
-  </si>
-  <si>
-    <t>uniform_scaling_q</t>
-  </si>
-  <si>
     <t>variable_trajectory_group_trajectory_type</t>
   </si>
   <si>
@@ -42,6 +51,114 @@
   </si>
   <si>
     <t>min_35</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
   </si>
   <si>
     <t>Economy</t>
@@ -472,121 +589,121 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>7</v>
-      </c>
-      <c r="R1" s="1">
-        <v>8</v>
-      </c>
-      <c r="S1" s="1">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="1">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="1">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="1">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="W1" s="1">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="1">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" s="1">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="1">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AD1" s="1">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AE1" s="1">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AF1" s="1">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AG1" s="1">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AH1" s="1">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AI1" s="1">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AJ1" s="1">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AK1" s="1">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AL1" s="1">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AM1" s="1">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AN1" s="1">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AO1" s="1">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AP1" s="1">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AQ1" s="1">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="1">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AS1" s="1">
+      <c r="AJ1" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:45">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -705,10 +822,10 @@
     </row>
     <row r="3" spans="1:45">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -827,10 +944,10 @@
     </row>
     <row r="4" spans="1:45">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -949,10 +1066,10 @@
     </row>
     <row r="5" spans="1:45">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1071,10 +1188,10 @@
     </row>
     <row r="6" spans="1:45">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -1086,117 +1203,117 @@
         <v>1</v>
       </c>
       <c r="K6">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="M6">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="N6">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="O6">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="P6">
-        <v>0.9399999999999999</v>
+        <v>1</v>
       </c>
       <c r="Q6">
-        <v>0.93</v>
+        <v>1</v>
       </c>
       <c r="R6">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="S6">
-        <v>0.91</v>
+        <v>1</v>
       </c>
       <c r="T6">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="U6">
-        <v>0.89</v>
+        <v>1</v>
       </c>
       <c r="V6">
-        <v>0.88</v>
+        <v>1</v>
       </c>
       <c r="W6">
-        <v>0.87</v>
+        <v>1</v>
       </c>
       <c r="X6">
-        <v>0.86</v>
+        <v>1</v>
       </c>
       <c r="Y6">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="Z6">
-        <v>0.84</v>
+        <v>1</v>
       </c>
       <c r="AA6">
-        <v>0.83</v>
+        <v>1</v>
       </c>
       <c r="AB6">
-        <v>0.82</v>
+        <v>1</v>
       </c>
       <c r="AC6">
-        <v>0.8100000000000001</v>
+        <v>1</v>
       </c>
       <c r="AD6">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AE6">
-        <v>0.79</v>
+        <v>1</v>
       </c>
       <c r="AF6">
-        <v>0.78</v>
+        <v>1</v>
       </c>
       <c r="AG6">
-        <v>0.77</v>
+        <v>1</v>
       </c>
       <c r="AH6">
-        <v>0.76</v>
+        <v>1</v>
       </c>
       <c r="AI6">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AJ6">
-        <v>0.74</v>
+        <v>1</v>
       </c>
       <c r="AK6">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="AL6">
-        <v>0.72</v>
+        <v>1</v>
       </c>
       <c r="AM6">
-        <v>0.71</v>
+        <v>1</v>
       </c>
       <c r="AN6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AO6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AP6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AQ6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AR6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AS6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:45">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -1315,10 +1432,10 @@
     </row>
     <row r="8" spans="1:45">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1437,10 +1554,10 @@
     </row>
     <row r="9" spans="1:45">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -1559,10 +1676,10 @@
     </row>
     <row r="10" spans="1:45">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -1571,120 +1688,120 @@
         <v>1</v>
       </c>
       <c r="J10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="K10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="L10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="M10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="N10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="O10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="P10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="Q10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="R10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="S10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="T10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="U10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="V10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="W10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="X10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="Y10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="Z10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="AA10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="AB10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="AC10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="AD10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="AE10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="AF10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="AG10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="AH10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="AI10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="AJ10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="AK10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="AL10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="AM10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="AN10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="AO10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="AP10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="AQ10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="AR10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
       <c r="AS10">
-        <v>3.919</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="11" spans="1:45">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -1693,234 +1810,778 @@
         <v>1</v>
       </c>
       <c r="J11">
-        <v>6899489.43177</v>
+        <v>1270673.58425</v>
       </c>
       <c r="K11">
-        <v>6946296.94596</v>
+        <v>1281946.4346</v>
       </c>
       <c r="L11">
-        <v>7005789.8172</v>
+        <v>1293261.57585</v>
       </c>
       <c r="M11">
-        <v>7067388.31645</v>
+        <v>1304619.008</v>
       </c>
       <c r="N11">
-        <v>7120116.28262</v>
+        <v>1330724.4091</v>
       </c>
       <c r="O11">
-        <v>7155879.73738</v>
+        <v>1348317.33</v>
       </c>
       <c r="P11">
-        <v>6800953.92641392</v>
+        <v>1328499.46483333</v>
       </c>
       <c r="Q11">
-        <v>6778708.36952214</v>
+        <v>1308206.67733333</v>
       </c>
       <c r="R11">
-        <v>6756462.81263036</v>
+        <v>1287425.5225</v>
       </c>
       <c r="S11">
-        <v>6734217.25573858</v>
+        <v>1266144.704</v>
       </c>
       <c r="T11">
-        <v>6711971.698846799</v>
+        <v>1244362.12916667</v>
       </c>
       <c r="U11">
-        <v>6679338.55338464</v>
+        <v>1222095.888</v>
       </c>
       <c r="V11">
-        <v>6646705.40792248</v>
+        <v>1199322.599</v>
       </c>
       <c r="W11">
-        <v>6614072.26246032</v>
+        <v>1176036.76166667</v>
       </c>
       <c r="X11">
-        <v>6581439.11699816</v>
+        <v>1152236.1915</v>
       </c>
       <c r="Y11">
-        <v>6548805.971536</v>
+        <v>1127922.22</v>
       </c>
       <c r="Z11">
-        <v>6505455.263050499</v>
+        <v>1103099.38633333</v>
       </c>
       <c r="AA11">
-        <v>6462104.554565</v>
+        <v>1077775.762</v>
       </c>
       <c r="AB11">
-        <v>6418753.846079499</v>
+        <v>1051962.95966667</v>
       </c>
       <c r="AC11">
-        <v>6375403.137594</v>
+        <v>1025675.07466667</v>
       </c>
       <c r="AD11">
-        <v>6332052.4291085</v>
+        <v>998926.775</v>
       </c>
       <c r="AE11">
-        <v>6279942.78738112</v>
+        <v>971734.296</v>
       </c>
       <c r="AF11">
-        <v>6227833.14565374</v>
+        <v>944114.411333333</v>
       </c>
       <c r="AG11">
-        <v>6175723.50392636</v>
+        <v>916083.03</v>
       </c>
       <c r="AH11">
-        <v>6123613.86219898</v>
+        <v>887656.569833333</v>
       </c>
       <c r="AI11">
-        <v>6071504.220471599</v>
+        <v>858850.933333333</v>
       </c>
       <c r="AJ11">
-        <v>6011427.33428911</v>
+        <v>829681.9125</v>
       </c>
       <c r="AK11">
-        <v>5951350.44810661</v>
+        <v>800165.333333333</v>
       </c>
       <c r="AL11">
-        <v>5891273.56192411</v>
+        <v>770315.981</v>
       </c>
       <c r="AM11">
-        <v>5831196.67574161</v>
+        <v>740149.213</v>
       </c>
       <c r="AN11">
-        <v>5771119.78955911</v>
+        <v>709679.380833333</v>
       </c>
       <c r="AO11">
-        <v>5704147.56278013</v>
+        <v>678919.5820000001</v>
       </c>
       <c r="AP11">
-        <v>5637175.33600115</v>
+        <v>647877.7755</v>
       </c>
       <c r="AQ11">
-        <v>5570203.10922217</v>
+        <v>616562.955666666</v>
       </c>
       <c r="AR11">
-        <v>5503230.88244318</v>
+        <v>584982.686166666</v>
       </c>
       <c r="AS11">
-        <v>5436258.6556642</v>
+        <v>553142.3</v>
       </c>
     </row>
     <row r="12" spans="1:45">
       <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>3324890.91575</v>
+      </c>
+      <c r="K12">
+        <v>3326056.5654</v>
+      </c>
+      <c r="L12">
+        <v>3327179.92415</v>
+      </c>
+      <c r="M12">
+        <v>3328260.992</v>
+      </c>
+      <c r="N12">
+        <v>3366502.5909</v>
+      </c>
+      <c r="O12">
+        <v>3382620.67</v>
+      </c>
+      <c r="P12">
+        <v>3435993.53516667</v>
+      </c>
+      <c r="Q12">
+        <v>3489617.32266667</v>
+      </c>
+      <c r="R12">
+        <v>3543439.4775</v>
+      </c>
+      <c r="S12">
+        <v>3597407.296</v>
+      </c>
+      <c r="T12">
+        <v>3651488.87083333</v>
+      </c>
+      <c r="U12">
+        <v>3705710.112</v>
+      </c>
+      <c r="V12">
+        <v>3759971.401</v>
+      </c>
+      <c r="W12">
+        <v>3814218.23833333</v>
+      </c>
+      <c r="X12">
+        <v>3868400.8085</v>
+      </c>
+      <c r="Y12">
+        <v>3922475.78</v>
+      </c>
+      <c r="Z12">
+        <v>3976406.61366667</v>
+      </c>
+      <c r="AA12">
+        <v>4030166.238</v>
+      </c>
+      <c r="AB12">
+        <v>4083739.04033333</v>
+      </c>
+      <c r="AC12">
+        <v>4137118.92533333</v>
+      </c>
+      <c r="AD12">
+        <v>4190303.225</v>
+      </c>
+      <c r="AE12">
+        <v>4243297.704</v>
+      </c>
+      <c r="AF12">
+        <v>4296113.58866667</v>
+      </c>
+      <c r="AG12">
+        <v>4348761.97</v>
+      </c>
+      <c r="AH12">
+        <v>4401260.43016667</v>
+      </c>
+      <c r="AI12">
+        <v>4453629.06666667</v>
+      </c>
+      <c r="AJ12">
+        <v>4505893.0875</v>
+      </c>
+      <c r="AK12">
+        <v>4558084.66666667</v>
+      </c>
+      <c r="AL12">
+        <v>4610238.019</v>
+      </c>
+      <c r="AM12">
+        <v>4662399.787</v>
+      </c>
+      <c r="AN12">
+        <v>4714621.61916667</v>
+      </c>
+      <c r="AO12">
+        <v>4766959.418</v>
+      </c>
+      <c r="AP12">
+        <v>4819445.2245</v>
+      </c>
+      <c r="AQ12">
+        <v>4872128.04433333</v>
+      </c>
+      <c r="AR12">
+        <v>4925058.31383333</v>
+      </c>
+      <c r="AS12">
+        <v>4978280.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>23571249.56823</v>
-      </c>
-      <c r="K12">
-        <v>23979739.05404</v>
-      </c>
-      <c r="L12">
-        <v>24438509.1828</v>
-      </c>
-      <c r="M12">
-        <v>24921876.68355</v>
-      </c>
-      <c r="N12">
-        <v>25390345.71738</v>
-      </c>
-      <c r="O12">
-        <v>25815966.26262</v>
-      </c>
-      <c r="P12">
-        <v>24816008.2895861</v>
-      </c>
-      <c r="Q12">
-        <v>25016246.8724779</v>
-      </c>
-      <c r="R12">
-        <v>25216485.4553696</v>
-      </c>
-      <c r="S12">
-        <v>25416724.0382614</v>
-      </c>
-      <c r="T12">
-        <v>25616962.6211532</v>
-      </c>
-      <c r="U12">
-        <v>25792089.3986154</v>
-      </c>
-      <c r="V12">
-        <v>25967216.1760775</v>
-      </c>
-      <c r="W12">
-        <v>26142342.9535397</v>
-      </c>
-      <c r="X12">
-        <v>26317469.7310018</v>
-      </c>
-      <c r="Y12">
-        <v>26492596.508464</v>
-      </c>
-      <c r="Z12">
-        <v>26635882.34094949</v>
-      </c>
-      <c r="AA12">
-        <v>26779168.173435</v>
-      </c>
-      <c r="AB12">
-        <v>26922454.0059205</v>
-      </c>
-      <c r="AC12">
-        <v>27065739.838406</v>
-      </c>
-      <c r="AD12">
-        <v>27209025.6708915</v>
-      </c>
-      <c r="AE12">
-        <v>27322729.8286189</v>
-      </c>
-      <c r="AF12">
-        <v>27436433.9863463</v>
-      </c>
-      <c r="AG12">
-        <v>27550138.1440736</v>
-      </c>
-      <c r="AH12">
-        <v>27663842.301801</v>
-      </c>
-      <c r="AI12">
-        <v>27777546.4595284</v>
-      </c>
-      <c r="AJ12">
-        <v>27859163.6137109</v>
-      </c>
-      <c r="AK12">
-        <v>27940780.7678934</v>
-      </c>
-      <c r="AL12">
-        <v>28022397.9220759</v>
-      </c>
-      <c r="AM12">
-        <v>28104015.0762584</v>
-      </c>
-      <c r="AN12">
-        <v>28185632.2304409</v>
-      </c>
-      <c r="AO12">
-        <v>28233720.2992199</v>
-      </c>
-      <c r="AP12">
-        <v>28281808.3679989</v>
-      </c>
-      <c r="AQ12">
-        <v>28329896.4367778</v>
-      </c>
-      <c r="AR12">
-        <v>28377984.5055568</v>
-      </c>
-      <c r="AS12">
-        <v>28426072.5743358</v>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0.9833333333333334</v>
+      </c>
+      <c r="Q2">
+        <v>0.9666666666666667</v>
+      </c>
+      <c r="R2">
+        <v>0.9500000000000001</v>
+      </c>
+      <c r="S2">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="T2">
+        <v>0.9166666666666667</v>
+      </c>
+      <c r="U2">
+        <v>0.9</v>
+      </c>
+      <c r="V2">
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="W2">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="X2">
+        <v>0.85</v>
+      </c>
+      <c r="Y2">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="Z2">
+        <v>0.8166666666666667</v>
+      </c>
+      <c r="AA2">
+        <v>0.8</v>
+      </c>
+      <c r="AB2">
+        <v>0.7833333333333333</v>
+      </c>
+      <c r="AC2">
+        <v>0.7666666666666666</v>
+      </c>
+      <c r="AD2">
+        <v>0.75</v>
+      </c>
+      <c r="AE2">
+        <v>0.7333333333333334</v>
+      </c>
+      <c r="AF2">
+        <v>0.7166666666666667</v>
+      </c>
+      <c r="AG2">
+        <v>0.7</v>
+      </c>
+      <c r="AH2">
+        <v>0.6833333333333333</v>
+      </c>
+      <c r="AI2">
+        <v>0.6666666666666667</v>
+      </c>
+      <c r="AJ2">
+        <v>0.65</v>
+      </c>
+      <c r="AK2">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="AL2">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="AM2">
+        <v>0.6</v>
+      </c>
+      <c r="AN2">
+        <v>0.5833333333333333</v>
+      </c>
+      <c r="AO2">
+        <v>0.5666666666666667</v>
+      </c>
+      <c r="AP2">
+        <v>0.55</v>
+      </c>
+      <c r="AQ2">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="AR2">
+        <v>0.5166666666666666</v>
+      </c>
+      <c r="AS2">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0.9833333333333334</v>
+      </c>
+      <c r="Q2">
+        <v>0.9666666666666667</v>
+      </c>
+      <c r="R2">
+        <v>0.9500000000000001</v>
+      </c>
+      <c r="S2">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="T2">
+        <v>0.9166666666666667</v>
+      </c>
+      <c r="U2">
+        <v>0.9</v>
+      </c>
+      <c r="V2">
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="W2">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="X2">
+        <v>0.85</v>
+      </c>
+      <c r="Y2">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="Z2">
+        <v>0.8166666666666667</v>
+      </c>
+      <c r="AA2">
+        <v>0.8</v>
+      </c>
+      <c r="AB2">
+        <v>0.7833333333333333</v>
+      </c>
+      <c r="AC2">
+        <v>0.7666666666666666</v>
+      </c>
+      <c r="AD2">
+        <v>0.75</v>
+      </c>
+      <c r="AE2">
+        <v>0.7333333333333334</v>
+      </c>
+      <c r="AF2">
+        <v>0.7166666666666667</v>
+      </c>
+      <c r="AG2">
+        <v>0.7</v>
+      </c>
+      <c r="AH2">
+        <v>0.6833333333333333</v>
+      </c>
+      <c r="AI2">
+        <v>0.6666666666666667</v>
+      </c>
+      <c r="AJ2">
+        <v>0.65</v>
+      </c>
+      <c r="AK2">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="AL2">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="AM2">
+        <v>0.6</v>
+      </c>
+      <c r="AN2">
+        <v>0.5833333333333333</v>
+      </c>
+      <c r="AO2">
+        <v>0.5666666666666667</v>
+      </c>
+      <c r="AP2">
+        <v>0.55</v>
+      </c>
+      <c r="AQ2">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="AR2">
+        <v>0.5166666666666666</v>
+      </c>
+      <c r="AS2">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -1964,122 +2625,666 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>7</v>
-      </c>
-      <c r="R1" s="1">
-        <v>8</v>
-      </c>
-      <c r="S1" s="1">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="1">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="1">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="1">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="W1" s="1">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="1">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" s="1">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="1">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AD1" s="1">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AE1" s="1">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AF1" s="1">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AG1" s="1">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AH1" s="1">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AI1" s="1">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AJ1" s="1">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AK1" s="1">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AL1" s="1">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AM1" s="1">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AN1" s="1">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AO1" s="1">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AP1" s="1">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AQ1" s="1">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="1">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AS1" s="1">
+      <c r="AJ1" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:45">
       <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0.9833333333333334</v>
+      </c>
+      <c r="Q2">
+        <v>0.9666666666666667</v>
+      </c>
+      <c r="R2">
+        <v>0.9500000000000001</v>
+      </c>
+      <c r="S2">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="T2">
+        <v>0.9166666666666667</v>
+      </c>
+      <c r="U2">
+        <v>0.9</v>
+      </c>
+      <c r="V2">
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="W2">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="X2">
+        <v>0.85</v>
+      </c>
+      <c r="Y2">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="Z2">
+        <v>0.8166666666666667</v>
+      </c>
+      <c r="AA2">
+        <v>0.8</v>
+      </c>
+      <c r="AB2">
+        <v>0.7833333333333333</v>
+      </c>
+      <c r="AC2">
+        <v>0.7666666666666666</v>
+      </c>
+      <c r="AD2">
+        <v>0.75</v>
+      </c>
+      <c r="AE2">
+        <v>0.7333333333333334</v>
+      </c>
+      <c r="AF2">
+        <v>0.7166666666666667</v>
+      </c>
+      <c r="AG2">
+        <v>0.7</v>
+      </c>
+      <c r="AH2">
+        <v>0.6833333333333333</v>
+      </c>
+      <c r="AI2">
+        <v>0.6666666666666667</v>
+      </c>
+      <c r="AJ2">
+        <v>0.65</v>
+      </c>
+      <c r="AK2">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="AL2">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="AM2">
+        <v>0.6</v>
+      </c>
+      <c r="AN2">
+        <v>0.5833333333333333</v>
+      </c>
+      <c r="AO2">
+        <v>0.5666666666666667</v>
+      </c>
+      <c r="AP2">
+        <v>0.55</v>
+      </c>
+      <c r="AQ2">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="AR2">
+        <v>0.5166666666666666</v>
+      </c>
+      <c r="AS2">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
       <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0.9833333333333334</v>
+      </c>
+      <c r="Q2">
+        <v>0.9666666666666667</v>
+      </c>
+      <c r="R2">
+        <v>0.9500000000000001</v>
+      </c>
+      <c r="S2">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="T2">
+        <v>0.9166666666666667</v>
+      </c>
+      <c r="U2">
+        <v>0.9</v>
+      </c>
+      <c r="V2">
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="W2">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="X2">
+        <v>0.85</v>
+      </c>
+      <c r="Y2">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="Z2">
+        <v>0.8166666666666667</v>
+      </c>
+      <c r="AA2">
+        <v>0.8</v>
+      </c>
+      <c r="AB2">
+        <v>0.7833333333333333</v>
+      </c>
+      <c r="AC2">
+        <v>0.7666666666666666</v>
+      </c>
+      <c r="AD2">
+        <v>0.75</v>
+      </c>
+      <c r="AE2">
+        <v>0.7333333333333334</v>
+      </c>
+      <c r="AF2">
+        <v>0.7166666666666667</v>
+      </c>
+      <c r="AG2">
+        <v>0.7</v>
+      </c>
+      <c r="AH2">
+        <v>0.6833333333333333</v>
+      </c>
+      <c r="AI2">
+        <v>0.6666666666666667</v>
+      </c>
+      <c r="AJ2">
+        <v>0.65</v>
+      </c>
+      <c r="AK2">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="AL2">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="AM2">
+        <v>0.6</v>
+      </c>
+      <c r="AN2">
+        <v>0.5833333333333333</v>
+      </c>
+      <c r="AO2">
+        <v>0.5666666666666667</v>
+      </c>
+      <c r="AP2">
+        <v>0.55</v>
+      </c>
+      <c r="AQ2">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="AR2">
+        <v>0.5166666666666666</v>
+      </c>
+      <c r="AS2">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
       <c r="H2">
         <v>1</v>
       </c>
@@ -2090,106 +3295,1466 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="M2">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="N2">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="O2">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="P2">
-        <v>0.9253333333333333</v>
+        <v>0.9833333333333334</v>
       </c>
       <c r="Q2">
-        <v>0.9013333333333334</v>
+        <v>0.9666666666666667</v>
       </c>
       <c r="R2">
-        <v>0.8780000000000001</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="S2">
-        <v>0.8553333333333334</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="T2">
+        <v>0.9166666666666667</v>
+      </c>
+      <c r="U2">
+        <v>0.9</v>
+      </c>
+      <c r="V2">
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="W2">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="X2">
+        <v>0.85</v>
+      </c>
+      <c r="Y2">
         <v>0.8333333333333334</v>
       </c>
+      <c r="Z2">
+        <v>0.8166666666666667</v>
+      </c>
+      <c r="AA2">
+        <v>0.8</v>
+      </c>
+      <c r="AB2">
+        <v>0.7833333333333333</v>
+      </c>
+      <c r="AC2">
+        <v>0.7666666666666666</v>
+      </c>
+      <c r="AD2">
+        <v>0.75</v>
+      </c>
+      <c r="AE2">
+        <v>0.7333333333333334</v>
+      </c>
+      <c r="AF2">
+        <v>0.7166666666666667</v>
+      </c>
+      <c r="AG2">
+        <v>0.7</v>
+      </c>
+      <c r="AH2">
+        <v>0.6833333333333333</v>
+      </c>
+      <c r="AI2">
+        <v>0.6666666666666667</v>
+      </c>
+      <c r="AJ2">
+        <v>0.65</v>
+      </c>
+      <c r="AK2">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="AL2">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="AM2">
+        <v>0.6</v>
+      </c>
+      <c r="AN2">
+        <v>0.5833333333333333</v>
+      </c>
+      <c r="AO2">
+        <v>0.5666666666666667</v>
+      </c>
+      <c r="AP2">
+        <v>0.55</v>
+      </c>
+      <c r="AQ2">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="AR2">
+        <v>0.5166666666666666</v>
+      </c>
+      <c r="AS2">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0.9833333333333334</v>
+      </c>
+      <c r="Q2">
+        <v>0.9666666666666667</v>
+      </c>
+      <c r="R2">
+        <v>0.9500000000000001</v>
+      </c>
+      <c r="S2">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="T2">
+        <v>0.9166666666666667</v>
+      </c>
       <c r="U2">
-        <v>0.8120000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="V2">
-        <v>0.7913333333333333</v>
+        <v>0.8833333333333333</v>
       </c>
       <c r="W2">
-        <v>0.7713333333333333</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="X2">
-        <v>0.752</v>
+        <v>0.85</v>
       </c>
       <c r="Y2">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="Z2">
+        <v>0.8166666666666667</v>
+      </c>
+      <c r="AA2">
+        <v>0.8</v>
+      </c>
+      <c r="AB2">
+        <v>0.7833333333333333</v>
+      </c>
+      <c r="AC2">
+        <v>0.7666666666666666</v>
+      </c>
+      <c r="AD2">
+        <v>0.75</v>
+      </c>
+      <c r="AE2">
         <v>0.7333333333333334</v>
       </c>
+      <c r="AF2">
+        <v>0.7166666666666667</v>
+      </c>
+      <c r="AG2">
+        <v>0.7</v>
+      </c>
+      <c r="AH2">
+        <v>0.6833333333333333</v>
+      </c>
+      <c r="AI2">
+        <v>0.6666666666666667</v>
+      </c>
+      <c r="AJ2">
+        <v>0.65</v>
+      </c>
+      <c r="AK2">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="AL2">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="AM2">
+        <v>0.6</v>
+      </c>
+      <c r="AN2">
+        <v>0.5833333333333333</v>
+      </c>
+      <c r="AO2">
+        <v>0.5666666666666667</v>
+      </c>
+      <c r="AP2">
+        <v>0.55</v>
+      </c>
+      <c r="AQ2">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="AR2">
+        <v>0.5166666666666666</v>
+      </c>
+      <c r="AS2">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0.9833333333333334</v>
+      </c>
+      <c r="Q2">
+        <v>0.9666666666666667</v>
+      </c>
+      <c r="R2">
+        <v>0.9500000000000001</v>
+      </c>
+      <c r="S2">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="T2">
+        <v>0.9166666666666667</v>
+      </c>
+      <c r="U2">
+        <v>0.9</v>
+      </c>
+      <c r="V2">
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="W2">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="X2">
+        <v>0.85</v>
+      </c>
+      <c r="Y2">
+        <v>0.8333333333333334</v>
+      </c>
       <c r="Z2">
-        <v>0.7153333333333333</v>
+        <v>0.8166666666666667</v>
       </c>
       <c r="AA2">
-        <v>0.698</v>
+        <v>0.8</v>
       </c>
       <c r="AB2">
-        <v>0.6813333333333333</v>
+        <v>0.7833333333333333</v>
       </c>
       <c r="AC2">
-        <v>0.6653333333333333</v>
+        <v>0.7666666666666666</v>
       </c>
       <c r="AD2">
+        <v>0.75</v>
+      </c>
+      <c r="AE2">
+        <v>0.7333333333333334</v>
+      </c>
+      <c r="AF2">
+        <v>0.7166666666666667</v>
+      </c>
+      <c r="AG2">
+        <v>0.7</v>
+      </c>
+      <c r="AH2">
+        <v>0.6833333333333333</v>
+      </c>
+      <c r="AI2">
+        <v>0.6666666666666667</v>
+      </c>
+      <c r="AJ2">
         <v>0.65</v>
       </c>
+      <c r="AK2">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="AL2">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="AM2">
+        <v>0.6</v>
+      </c>
+      <c r="AN2">
+        <v>0.5833333333333333</v>
+      </c>
+      <c r="AO2">
+        <v>0.5666666666666667</v>
+      </c>
+      <c r="AP2">
+        <v>0.55</v>
+      </c>
+      <c r="AQ2">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="AR2">
+        <v>0.5166666666666666</v>
+      </c>
+      <c r="AS2">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0.9833333333333334</v>
+      </c>
+      <c r="Q2">
+        <v>0.9666666666666667</v>
+      </c>
+      <c r="R2">
+        <v>0.9500000000000001</v>
+      </c>
+      <c r="S2">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="T2">
+        <v>0.9166666666666667</v>
+      </c>
+      <c r="U2">
+        <v>0.9</v>
+      </c>
+      <c r="V2">
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="W2">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="X2">
+        <v>0.85</v>
+      </c>
+      <c r="Y2">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="Z2">
+        <v>0.8166666666666667</v>
+      </c>
+      <c r="AA2">
+        <v>0.8</v>
+      </c>
+      <c r="AB2">
+        <v>0.7833333333333333</v>
+      </c>
+      <c r="AC2">
+        <v>0.7666666666666666</v>
+      </c>
+      <c r="AD2">
+        <v>0.75</v>
+      </c>
       <c r="AE2">
-        <v>0.6353333333333333</v>
+        <v>0.7333333333333334</v>
       </c>
       <c r="AF2">
-        <v>0.6213333333333333</v>
+        <v>0.7166666666666667</v>
       </c>
       <c r="AG2">
-        <v>0.6080000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="AH2">
-        <v>0.5953333333333333</v>
+        <v>0.6833333333333333</v>
       </c>
       <c r="AI2">
+        <v>0.6666666666666667</v>
+      </c>
+      <c r="AJ2">
+        <v>0.65</v>
+      </c>
+      <c r="AK2">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="AL2">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="AM2">
+        <v>0.6</v>
+      </c>
+      <c r="AN2">
         <v>0.5833333333333333</v>
       </c>
+      <c r="AO2">
+        <v>0.5666666666666667</v>
+      </c>
+      <c r="AP2">
+        <v>0.55</v>
+      </c>
+      <c r="AQ2">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="AR2">
+        <v>0.5166666666666666</v>
+      </c>
+      <c r="AS2">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0.9833333333333334</v>
+      </c>
+      <c r="Q2">
+        <v>0.9666666666666667</v>
+      </c>
+      <c r="R2">
+        <v>0.9500000000000001</v>
+      </c>
+      <c r="S2">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="T2">
+        <v>0.9166666666666667</v>
+      </c>
+      <c r="U2">
+        <v>0.9</v>
+      </c>
+      <c r="V2">
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="W2">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="X2">
+        <v>0.85</v>
+      </c>
+      <c r="Y2">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="Z2">
+        <v>0.8166666666666667</v>
+      </c>
+      <c r="AA2">
+        <v>0.8</v>
+      </c>
+      <c r="AB2">
+        <v>0.7833333333333333</v>
+      </c>
+      <c r="AC2">
+        <v>0.7666666666666666</v>
+      </c>
+      <c r="AD2">
+        <v>0.75</v>
+      </c>
+      <c r="AE2">
+        <v>0.7333333333333334</v>
+      </c>
+      <c r="AF2">
+        <v>0.7166666666666667</v>
+      </c>
+      <c r="AG2">
+        <v>0.7</v>
+      </c>
+      <c r="AH2">
+        <v>0.6833333333333333</v>
+      </c>
+      <c r="AI2">
+        <v>0.6666666666666667</v>
+      </c>
       <c r="AJ2">
-        <v>0.5720000000000001</v>
+        <v>0.65</v>
       </c>
       <c r="AK2">
-        <v>0.5613333333333334</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="AL2">
-        <v>0.5513333333333333</v>
+        <v>0.6166666666666667</v>
       </c>
       <c r="AM2">
-        <v>0.542</v>
+        <v>0.6</v>
       </c>
       <c r="AN2">
+        <v>0.5833333333333333</v>
+      </c>
+      <c r="AO2">
+        <v>0.5666666666666667</v>
+      </c>
+      <c r="AP2">
+        <v>0.55</v>
+      </c>
+      <c r="AQ2">
         <v>0.5333333333333333</v>
       </c>
+      <c r="AR2">
+        <v>0.5166666666666666</v>
+      </c>
+      <c r="AS2">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0.9833333333333334</v>
+      </c>
+      <c r="Q2">
+        <v>0.9666666666666667</v>
+      </c>
+      <c r="R2">
+        <v>0.9500000000000001</v>
+      </c>
+      <c r="S2">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="T2">
+        <v>0.9166666666666667</v>
+      </c>
+      <c r="U2">
+        <v>0.9</v>
+      </c>
+      <c r="V2">
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="W2">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="X2">
+        <v>0.85</v>
+      </c>
+      <c r="Y2">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="Z2">
+        <v>0.8166666666666667</v>
+      </c>
+      <c r="AA2">
+        <v>0.8</v>
+      </c>
+      <c r="AB2">
+        <v>0.7833333333333333</v>
+      </c>
+      <c r="AC2">
+        <v>0.7666666666666666</v>
+      </c>
+      <c r="AD2">
+        <v>0.75</v>
+      </c>
+      <c r="AE2">
+        <v>0.7333333333333334</v>
+      </c>
+      <c r="AF2">
+        <v>0.7166666666666667</v>
+      </c>
+      <c r="AG2">
+        <v>0.7</v>
+      </c>
+      <c r="AH2">
+        <v>0.6833333333333333</v>
+      </c>
+      <c r="AI2">
+        <v>0.6666666666666667</v>
+      </c>
+      <c r="AJ2">
+        <v>0.65</v>
+      </c>
+      <c r="AK2">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="AL2">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="AM2">
+        <v>0.6</v>
+      </c>
+      <c r="AN2">
+        <v>0.5833333333333333</v>
+      </c>
       <c r="AO2">
-        <v>0.5266666666666666</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="AP2">
-        <v>0.52</v>
+        <v>0.55</v>
       </c>
       <c r="AQ2">
-        <v>0.5133333333333333</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="AR2">
-        <v>0.5066666666666667</v>
+        <v>0.5166666666666666</v>
       </c>
       <c r="AS2">
         <v>0.5</v>

</xml_diff>